<commit_message>
update connection delete excel
</commit_message>
<xml_diff>
--- a/Test_Suite/rdp_delete.xlsx
+++ b/Test_Suite/rdp_delete.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\Test_Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E76AF1E-9E76-4CC3-97A5-B82D5FFC6F9C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADA371C-1DB3-425B-97BF-1DDB355190B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32160" yWindow="348" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>CheckPoint</t>
   </si>
@@ -104,68 +104,6 @@
         <family val="3"/>
       </rPr>
       <t>'delete'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'conn'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Shell_RDP().utils(</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'standardRDP'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF008080"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>'exist'</t>
     </r>
     <r>
       <rPr>
@@ -305,10 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -596,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,142 +566,101 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>7</v>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="3"/>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B39" s="3"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="2"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C47" s="4"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="4"/>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="4"/>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C51" s="4"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C52" s="4"/>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C54" s="4"/>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C55" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>